<commit_message>
feat: Enhance metadata extraction by adding raw DataFrame parameter and updating metadata keys for improved sheet handling
</commit_message>
<xml_diff>
--- a/outputs/budget_tables_concatenated.xlsx
+++ b/outputs/budget_tables_concatenated.xlsx
@@ -47385,18 +47385,18 @@
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ITAÚ UNIBANCO S/A - AG. 4830 - SANTOS - BOQUEIRÃO - SP</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ITAÚ UNIBANCO S/A - AG. 4830 - SANTOS - BOQUEIRÃO - SP</t>
+          <t>M2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>M2</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>

</xml_diff>